<commit_message>
try to fix render markdown
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/program_preferred_by_millionaire_tax_vote_country.xlsx
+++ b/xlsx/country_comparison/program_preferred_by_millionaire_tax_vote_country.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">y</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;All&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*All*</t>
   </si>
   <si>
     <t xml:space="preserve">Left</t>
@@ -431,7 +434,7 @@
         <v>0.0603369023918985</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -448,7 +451,7 @@
         <v>0.154991283166542</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -465,7 +468,7 @@
         <v>0.0102520419636565</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -482,12 +485,12 @@
         <v>0.0680276010868375</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="n">
         <v>0.0465731370810216</v>
@@ -499,12 +502,12 @@
         <v>0.071388638073594</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n">
         <v>0.127404494753902</v>
@@ -516,12 +519,12 @@
         <v>0.173357263478352</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
         <v>-0.0137758450767718</v>
@@ -533,12 +536,12 @@
         <v>0.02189574627848</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="n">
         <v>0.0696097657082823</v>
@@ -550,12 +553,12 @@
         <v>0.121049654861424</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="n">
         <v>0.013420084143708</v>
@@ -567,12 +570,12 @@
         <v>0.0704507545106575</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="n">
         <v>0.163506162024661</v>
@@ -584,12 +587,12 @@
         <v>0.284860136446389</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
         <v>-0.0745597824524039</v>
@@ -601,12 +604,12 @@
         <v>0.00322460706046568</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>0.0440008700361147</v>
@@ -618,12 +621,12 @@
         <v>0.153486951481055</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>0.0569667855655538</v>
@@ -635,12 +638,12 @@
         <v>0.109583624012725</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B15" t="n">
         <v>0.0659471240980055</v>
@@ -652,12 +655,12 @@
         <v>0.152414495004557</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" t="n">
         <v>0.0420427490991278</v>
@@ -669,12 +672,12 @@
         <v>0.115830082456702</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="n">
         <v>0.106517429484949</v>
@@ -686,12 +689,12 @@
         <v>0.262553493818095</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" t="n">
         <v>0.0443478060551181</v>
@@ -703,12 +706,12 @@
         <v>0.106774553136503</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" t="n">
         <v>0.119205559811995</v>
@@ -720,12 +723,12 @@
         <v>0.218581928511769</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" t="n">
         <v>-0.0562340313072508</v>
@@ -737,12 +740,12 @@
         <v>0.0446797350568945</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" t="n">
         <v>0.062045527592155</v>
@@ -754,12 +757,12 @@
         <v>0.192422461466832</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22" t="n">
         <v>0.0498913264863574</v>
@@ -771,12 +774,12 @@
         <v>0.124979330763766</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23" t="n">
         <v>0.0209032692682398</v>
@@ -788,12 +791,12 @@
         <v>0.350155444550101</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24" t="n">
         <v>0.0647744067478856</v>
@@ -805,12 +808,12 @@
         <v>0.15766733734727</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" t="n">
         <v>0.0235743880088169</v>
@@ -822,12 +825,12 @@
         <v>0.16475502747135</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" t="n">
         <v>0.0792715060759077</v>
@@ -839,12 +842,12 @@
         <v>0.151224795292894</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" t="n">
         <v>0.183435976797437</v>
@@ -856,12 +859,12 @@
         <v>0.30586953239101</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B28" t="n">
         <v>-0.00249226313924833</v>
@@ -873,12 +876,12 @@
         <v>0.112635319004905</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" t="n">
         <v>0.0671222011710891</v>
@@ -890,12 +893,12 @@
         <v>0.201530842655811</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B30" t="n">
         <v>0.0461112468869427</v>
@@ -907,12 +910,12 @@
         <v>0.107823851766728</v>
       </c>
       <c r="E30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B31" t="n">
         <v>0.164292921240961</v>
@@ -924,12 +927,12 @@
         <v>0.271082091716684</v>
       </c>
       <c r="E31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B32" t="n">
         <v>-0.0770115323775564</v>
@@ -941,12 +944,12 @@
         <v>0.0144534036135903</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B33" t="n">
         <v>0.112378446213999</v>
@@ -958,12 +961,12 @@
         <v>0.240863344599851</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B34" t="n">
         <v>0.0128815133359225</v>
@@ -975,12 +978,12 @@
         <v>0.0927836393344068</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B35" t="n">
         <v>0.0000835166697395027</v>
@@ -992,12 +995,12 @@
         <v>0.208024977413496</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B36" t="n">
         <v>-0.0564745040254747</v>
@@ -1009,12 +1012,12 @@
         <v>0.051737294909373</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B37" t="n">
         <v>0.10753578576963</v>
@@ -1026,12 +1029,12 @@
         <v>0.245224317215406</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B38" t="n">
         <v>0.0328770242439968</v>
@@ -1043,12 +1046,12 @@
         <v>0.0699803283973505</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B39" t="n">
         <v>0.099488370636476</v>
@@ -1060,12 +1063,12 @@
         <v>0.177965349300314</v>
       </c>
       <c r="E39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B40" t="n">
         <v>0.0095152302348003</v>
@@ -1077,12 +1080,12 @@
         <v>0.062235141459281</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B41" t="n">
         <v>0.0151352460534197</v>
@@ -1094,12 +1097,12 @@
         <v>0.0849211604460325</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B42" t="n">
         <v>0.0443679478200813</v>
@@ -1111,12 +1114,12 @@
         <v>0.0746367717671793</v>
       </c>
       <c r="E42" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B43" t="n">
         <v>0.129837751330908</v>
@@ -1128,12 +1131,12 @@
         <v>0.176300427398495</v>
       </c>
       <c r="E43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B44" t="n">
         <v>-0.0302044720560949</v>
@@ -1145,12 +1148,12 @@
         <v>0.0197756235176154</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B45" t="n">
         <v>0.000989468184879495</v>
@@ -1162,7 +1165,7 @@
         <v>0.0652903723322032</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>